<commit_message>
Updated Sulu-ADS1299 bom and component files for assembly
</commit_message>
<xml_diff>
--- a/sulu-ads1299/sulu_ads1299_bom_final.xlsx
+++ b/sulu-ads1299/sulu_ads1299_bom_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-ads1299\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808BF6FE-A9CB-44B8-9402-C3F7B9F5355C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E4B972-1BC5-4945-A3E0-EDB78A8F2CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="2655" windowWidth="15270" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9240" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sulu_ads1299" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -438,6 +438,15 @@
   <si>
     <t>200 Ohms ±0.5% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thin Film</t>
     <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Populate</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -937,12 +946,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1299,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1314,11 +1324,12 @@
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1346,8 +1357,11 @@
       <c r="I1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1375,8 +1389,11 @@
       <c r="I2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1401,8 +1418,11 @@
       <c r="I3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1427,8 +1447,11 @@
       <c r="I4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -1450,8 +1473,11 @@
       <c r="I5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1476,8 +1502,11 @@
       <c r="I6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -1502,31 +1531,37 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="J7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>733910060</v>
       </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -1551,8 +1586,11 @@
       <c r="I9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1574,8 +1612,11 @@
       <c r="I10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1597,8 +1638,11 @@
       <c r="I11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -1620,8 +1664,11 @@
       <c r="I12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1643,8 +1690,11 @@
       <c r="I13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1666,8 +1716,11 @@
       <c r="I14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1689,8 +1742,11 @@
       <c r="I15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1709,8 +1765,11 @@
       <c r="I16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1738,22 +1797,28 @@
       <c r="I17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
+      <c r="J17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1">
+      <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1778,8 +1843,11 @@
       <c r="I19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -1804,8 +1872,11 @@
       <c r="I20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1830,8 +1901,11 @@
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -1856,8 +1930,11 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>112</v>
       </c>
@@ -1882,8 +1959,11 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -1908,8 +1988,11 @@
       <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -1933,6 +2016,9 @@
       </c>
       <c r="I25">
         <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sulu-ADS1299 filled in missing BoM entries, removed part list
</commit_message>
<xml_diff>
--- a/sulu-ads1299/sulu_ads1299_bom_final.xlsx
+++ b/sulu-ads1299/sulu_ads1299_bom_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-ads1299\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E4B972-1BC5-4945-A3E0-EDB78A8F2CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8374C59-1543-4353-A932-D6BC95276A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9240" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9240" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sulu_ads1299" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -447,6 +447,33 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>ABLIC Inc.</t>
+  </si>
+  <si>
+    <t>LM2775QDSGRQ1</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>RES 0 OHM</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>RES (NP)</t>
+  </si>
+  <si>
+    <t>CAP CER (NP)</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5</t>
+  </si>
+  <si>
+    <t>C21, C22, C23, C24, C25</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1328,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1309,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1361,62 +1388,44 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>136</v>
+    <row r="2" spans="1:10" s="3" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="I3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J3" t="s">
         <v>136</v>
@@ -1424,28 +1433,28 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J4" t="s">
         <v>136</v>
@@ -1453,25 +1462,28 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>129</v>
+      <c r="H5" t="s">
+        <v>70</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
         <v>136</v>
@@ -1479,28 +1491,25 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
-        <v>54</v>
+      <c r="H6" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
         <v>136</v>
@@ -1508,135 +1517,123 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="3">
         <v>733910060</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" t="s">
         <v>136</v>
@@ -1644,25 +1641,25 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>132</v>
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>131</v>
+      <c r="H12" t="s">
+        <v>31</v>
       </c>
       <c r="I12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J12" t="s">
         <v>136</v>
@@ -1670,100 +1667,73 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13">
-        <v>74438343022</v>
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>96</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>136</v>
+    <row r="14" spans="1:10" s="3" customFormat="1">
+      <c r="A14" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1">
+      <c r="A15" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>89</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="H16" t="s">
-        <v>52</v>
+      <c r="H16" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J16" t="s">
         <v>136</v>
@@ -1771,74 +1741,80 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>74438343022</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
-      <c r="G17" t="s">
-        <v>62</v>
-      </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1">
-      <c r="A18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="3">
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>137</v>
+      <c r="J18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1849,25 +1825,25 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="H20" t="s">
-        <v>92</v>
+      <c r="H20" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1878,25 +1854,28 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
+      <c r="G21" t="s">
+        <v>62</v>
+      </c>
       <c r="H21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1905,56 +1884,44 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" t="s">
-        <v>107</v>
-      </c>
-      <c r="I22">
+    <row r="22" spans="1:10" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="3">
         <v>1</v>
       </c>
-      <c r="J22" t="s">
-        <v>136</v>
+      <c r="J22" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1965,25 +1932,25 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1994,56 +1961,172 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H13" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
-    <hyperlink ref="H15" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>
-    <hyperlink ref="H14" r:id="rId3" xr:uid="{0B01DD8A-3997-4A8C-B042-D0235E7E2358}"/>
-    <hyperlink ref="H11" r:id="rId4" xr:uid="{E1F80F4E-F86A-4632-8550-92AA851DDFA0}"/>
-    <hyperlink ref="H10" r:id="rId5" xr:uid="{AED77D91-9A40-43A2-A4C6-D80D81896EDA}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{DA046B72-EBDF-4999-8536-8FDB28899EEA}"/>
-    <hyperlink ref="H2" r:id="rId7" xr:uid="{74E594FB-869E-4304-BA09-F1256497435B}"/>
-    <hyperlink ref="H21" r:id="rId8" xr:uid="{E3E06297-BCFB-4337-A5D7-EF69871C797A}"/>
-    <hyperlink ref="H6" r:id="rId9" xr:uid="{90261672-F139-440C-8B8C-17EB9F730C48}"/>
-    <hyperlink ref="H17" r:id="rId10" xr:uid="{BD7ED755-FC34-4D81-8BC9-0E8F7C10635C}"/>
-    <hyperlink ref="H7" r:id="rId11" xr:uid="{371CC253-C125-45F4-B084-8B33831407CC}"/>
-    <hyperlink ref="H4" r:id="rId12" xr:uid="{C04EB7A7-D999-4D0C-8F70-30E43677A7BB}"/>
-    <hyperlink ref="H3" r:id="rId13" xr:uid="{216F26A6-FF51-4197-9F8D-85A6BB14472C}"/>
-    <hyperlink ref="H20" r:id="rId14" xr:uid="{7145ECDF-EB7F-4BA6-BE13-5FB45BECF207}"/>
-    <hyperlink ref="H12" r:id="rId15" xr:uid="{9D3A25CC-75B8-47AA-B851-BE72F41215FB}"/>
-    <hyperlink ref="H16" r:id="rId16" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2775QDSGRQ1/9675908?utm_adgroup=Texas%20Instruments&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Focus%20Suppliers&amp;utm_term=&amp;utm_content=Texas%20Instruments&amp;gclid=Cj0KCQjwj7CZBhDHARIsAPPWv3c7aiWpXHenzAKn8sFqMkFxni_juonNmcSJ7Dx9oyr-PlFVMiiO4WoaAjmMEALw_wcB" xr:uid="{3357C052-7B51-4092-A76A-A3B0DF441934}"/>
-    <hyperlink ref="H9" r:id="rId17" xr:uid="{4B7FC37A-F345-4C96-864F-340BDED2421E}"/>
-    <hyperlink ref="H22" r:id="rId18" xr:uid="{70D4DCF0-D1F8-4A62-9B9C-724138118DCF}"/>
-    <hyperlink ref="H25" r:id="rId19" xr:uid="{7E384250-9D50-4A0D-AC23-DBEBE885B911}"/>
-    <hyperlink ref="H5" r:id="rId20" xr:uid="{29CF3033-1CEE-41DB-8629-4BB92A23F340}"/>
+    <hyperlink ref="H17" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
+    <hyperlink ref="H19" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>
+    <hyperlink ref="H18" r:id="rId3" xr:uid="{0B01DD8A-3997-4A8C-B042-D0235E7E2358}"/>
+    <hyperlink ref="H13" r:id="rId4" xr:uid="{E1F80F4E-F86A-4632-8550-92AA851DDFA0}"/>
+    <hyperlink ref="H12" r:id="rId5" xr:uid="{AED77D91-9A40-43A2-A4C6-D80D81896EDA}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{DA046B72-EBDF-4999-8536-8FDB28899EEA}"/>
+    <hyperlink ref="H3" r:id="rId7" xr:uid="{74E594FB-869E-4304-BA09-F1256497435B}"/>
+    <hyperlink ref="H25" r:id="rId8" xr:uid="{E3E06297-BCFB-4337-A5D7-EF69871C797A}"/>
+    <hyperlink ref="H7" r:id="rId9" xr:uid="{90261672-F139-440C-8B8C-17EB9F730C48}"/>
+    <hyperlink ref="H21" r:id="rId10" xr:uid="{BD7ED755-FC34-4D81-8BC9-0E8F7C10635C}"/>
+    <hyperlink ref="H8" r:id="rId11" xr:uid="{371CC253-C125-45F4-B084-8B33831407CC}"/>
+    <hyperlink ref="H5" r:id="rId12" xr:uid="{C04EB7A7-D999-4D0C-8F70-30E43677A7BB}"/>
+    <hyperlink ref="H4" r:id="rId13" xr:uid="{216F26A6-FF51-4197-9F8D-85A6BB14472C}"/>
+    <hyperlink ref="H24" r:id="rId14" xr:uid="{7145ECDF-EB7F-4BA6-BE13-5FB45BECF207}"/>
+    <hyperlink ref="H16" r:id="rId15" xr:uid="{9D3A25CC-75B8-47AA-B851-BE72F41215FB}"/>
+    <hyperlink ref="H20" r:id="rId16" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2775QDSGRQ1/9675908?utm_adgroup=Texas%20Instruments&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Focus%20Suppliers&amp;utm_term=&amp;utm_content=Texas%20Instruments&amp;gclid=Cj0KCQjwj7CZBhDHARIsAPPWv3c7aiWpXHenzAKn8sFqMkFxni_juonNmcSJ7Dx9oyr-PlFVMiiO4WoaAjmMEALw_wcB" xr:uid="{3357C052-7B51-4092-A76A-A3B0DF441934}"/>
+    <hyperlink ref="H11" r:id="rId17" xr:uid="{4B7FC37A-F345-4C96-864F-340BDED2421E}"/>
+    <hyperlink ref="H26" r:id="rId18" xr:uid="{70D4DCF0-D1F8-4A62-9B9C-724138118DCF}"/>
+    <hyperlink ref="H29" r:id="rId19" xr:uid="{7E384250-9D50-4A0D-AC23-DBEBE885B911}"/>
+    <hyperlink ref="H6" r:id="rId20" xr:uid="{29CF3033-1CEE-41DB-8629-4BB92A23F340}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>

</xml_diff>